<commit_message>
Fixed path error in logging function, log file is now stored in results folder.
</commit_message>
<xml_diff>
--- a/docs/Files/ElementContentMaterials_Tutorial.xlsx
+++ b/docs/Files/ElementContentMaterials_Tutorial.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -239,7 +239,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,6 +279,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -322,7 +328,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -629,29 +635,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.42578125" customWidth="1"/>
-    <col min="8" max="8" width="3.5703125" customWidth="1"/>
-    <col min="9" max="9" width="3.42578125" customWidth="1"/>
-    <col min="10" max="11" width="3.28515625" customWidth="1"/>
+    <col min="1" max="1" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.44140625" customWidth="1"/>
+    <col min="8" max="8" width="3.5546875" customWidth="1"/>
+    <col min="9" max="9" width="3.44140625" customWidth="1"/>
+    <col min="10" max="11" width="3.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -665,7 +671,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -679,7 +685,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
@@ -693,7 +699,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
@@ -707,7 +713,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
@@ -721,7 +727,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -735,7 +741,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
@@ -749,7 +755,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -763,7 +769,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>4</v>
       </c>
@@ -777,7 +783,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>5</v>
       </c>
@@ -791,7 +797,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>19</v>
       </c>
@@ -805,7 +811,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
@@ -819,7 +825,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>21</v>
       </c>
@@ -833,7 +839,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>7</v>
       </c>
@@ -850,7 +856,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>36</v>
       </c>
@@ -867,7 +873,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>8</v>
       </c>
@@ -887,7 +893,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>39</v>
       </c>
@@ -907,7 +913,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>35</v>
       </c>
@@ -915,7 +921,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="L20" s="1" t="s">
         <v>38</v>
       </c>
@@ -930,20 +936,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H421"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
@@ -963,8 +969,8 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B2" s="12" t="s">
@@ -973,9 +979,15 @@
       <c r="C2" s="10">
         <v>0.96</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="D2">
+        <v>0.92</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -984,10 +996,16 @@
       <c r="C3" s="10">
         <v>0.92</v>
       </c>
+      <c r="D3">
+        <v>0.85</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
       <c r="H3" s="10"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B4" s="12" t="s">
@@ -996,10 +1014,17 @@
       <c r="C4" s="10">
         <v>0.8</v>
       </c>
+      <c r="D4">
+        <f t="shared" ref="D3:D33" si="0">0.7*C4</f>
+        <v>0.55999999999999994</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
       <c r="H4" s="10"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B5" s="12" t="s">
@@ -1008,10 +1033,16 @@
       <c r="C5" s="10">
         <v>0.97</v>
       </c>
+      <c r="D5">
+        <v>0.92</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
       <c r="H5" s="10"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B6" s="12" t="s">
@@ -1020,10 +1051,18 @@
       <c r="C6" s="10">
         <v>0.5</v>
       </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0.35</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E3:E33" si="1">1.3*C6</f>
+        <v>0.65</v>
+      </c>
       <c r="H6" s="10"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B7" s="12" t="s">
@@ -1032,10 +1071,18 @@
       <c r="C7" s="10">
         <v>0.5</v>
       </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0.35</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>0.65</v>
+      </c>
       <c r="H7" s="10"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -1044,10 +1091,18 @@
       <c r="C8" s="10">
         <v>0.5</v>
       </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0.35</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>0.65</v>
+      </c>
       <c r="H8" s="10"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B9" s="12" t="s">
@@ -1056,10 +1111,18 @@
       <c r="C9" s="10">
         <v>1E-3</v>
       </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>1.3000000000000002E-3</v>
+      </c>
       <c r="H9" s="10"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B10" s="12" t="s">
@@ -1068,10 +1131,18 @@
       <c r="C10" s="10">
         <v>2E-3</v>
       </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>1.4E-3</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>2.6000000000000003E-3</v>
+      </c>
       <c r="H10" s="10"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B11" s="12" t="s">
@@ -1080,10 +1151,18 @@
       <c r="C11" s="10">
         <v>2.0000000000000001E-4</v>
       </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>1.3999999999999999E-4</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>2.6000000000000003E-4</v>
+      </c>
       <c r="H11" s="10"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B12" s="12" t="s">
@@ -1092,10 +1171,18 @@
       <c r="C12" s="10">
         <v>1E-4</v>
       </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>6.9999999999999994E-5</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>1.3000000000000002E-4</v>
+      </c>
       <c r="H12" s="10"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B13" s="12" t="s">
@@ -1104,9 +1191,17 @@
       <c r="C13" s="10">
         <v>1E-4</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>6.9999999999999994E-5</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>1.3000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B14" s="12" t="s">
@@ -1115,9 +1210,17 @@
       <c r="C14" s="10">
         <v>1E-4</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>6.9999999999999994E-5</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>1.3000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -1126,9 +1229,17 @@
       <c r="C15" s="10">
         <v>1E-4</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>6.9999999999999994E-5</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>1.3000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B16" s="12" t="s">
@@ -1137,9 +1248,17 @@
       <c r="C16" s="10">
         <v>2E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>1.4E-3</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>2.6000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B17" s="12" t="s">
@@ -1148,9 +1267,17 @@
       <c r="C17" s="10">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>6.9999999999999993E-3</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>1.3000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B18" s="12" t="s">
@@ -1159,9 +1286,17 @@
       <c r="C18" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B19" s="12" t="s">
@@ -1170,9 +1305,17 @@
       <c r="C19" s="10">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>2.0999999999999998E-2</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>3.9E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B20" s="12" t="s">
@@ -1181,9 +1324,17 @@
       <c r="C20" s="10">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>5.5999999999999994E-2</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>0.10400000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B21" s="12" t="s">
@@ -1192,9 +1343,17 @@
       <c r="C21" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B22" s="12" t="s">
@@ -1203,9 +1362,17 @@
       <c r="C22" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B23" s="12" t="s">
@@ -1214,9 +1381,17 @@
       <c r="C23" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B24" s="12" t="s">
@@ -1225,9 +1400,17 @@
       <c r="C24" s="10">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>0.35</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B25" s="12" t="s">
@@ -1236,9 +1419,17 @@
       <c r="C25" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B26" s="12" t="s">
@@ -1247,9 +1438,17 @@
       <c r="C26" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B27" s="12" t="s">
@@ -1258,9 +1457,17 @@
       <c r="C27" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B28" s="12" t="s">
@@ -1269,9 +1476,17 @@
       <c r="C28" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B29" s="12" t="s">
@@ -1280,9 +1495,17 @@
       <c r="C29" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B30" s="12" t="s">
@@ -1291,9 +1514,17 @@
       <c r="C30" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B31" s="12" t="s">
@@ -1302,9 +1533,17 @@
       <c r="C31" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B32" s="12" t="s">
@@ -1313,9 +1552,17 @@
       <c r="C32" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B33" s="12" t="s">
@@ -1324,1557 +1571,1175 @@
       <c r="C33" s="10">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
+      <c r="D33">
+        <v>0.98</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C34" s="10"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="10"/>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C35" s="10"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="10"/>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C36" s="10"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="10"/>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C37" s="10"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="10"/>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C38" s="10"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="10"/>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C39" s="10"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="10"/>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C40" s="10"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="10"/>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C41" s="10"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="10"/>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C42" s="10"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="10"/>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C43" s="10"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="10"/>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C44" s="10"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="10"/>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C45" s="10"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="10"/>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C46" s="10"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="10"/>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C47" s="10"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="10"/>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C48" s="10"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="10"/>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C49" s="10"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="10"/>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C50" s="10"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="10"/>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C51" s="10"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="10"/>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C52" s="10"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="10"/>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C53" s="10"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="10"/>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C54" s="10"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="10"/>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C55" s="10"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="10"/>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C56" s="10"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="10"/>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C57" s="10"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="10"/>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C58" s="10"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="10"/>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C59" s="10"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="10"/>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C60" s="10"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="10"/>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C61" s="10"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="10"/>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C62" s="10"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="10"/>
+    <row r="63" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C63" s="10"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="10"/>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C64" s="10"/>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="10"/>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C65" s="10"/>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="10"/>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C66" s="10"/>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="10"/>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C67" s="10"/>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="10"/>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C68" s="10"/>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="10"/>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C69" s="10"/>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="10"/>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C70" s="10"/>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="10"/>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C71" s="10"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="10"/>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C72" s="10"/>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="10"/>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C73" s="10"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="10"/>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C74" s="10"/>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="10"/>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C75" s="10"/>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="10"/>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C76" s="10"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="10"/>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C77" s="10"/>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="10"/>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C78" s="10"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="10"/>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C79" s="10"/>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="10"/>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C80" s="10"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="10"/>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C81" s="10"/>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="10"/>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C82" s="10"/>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="10"/>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C83" s="10"/>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="10"/>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C84" s="10"/>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="10"/>
+    <row r="85" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C85" s="10"/>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="10"/>
+    <row r="86" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C86" s="10"/>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="10"/>
+    <row r="87" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C87" s="10"/>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="10"/>
+    <row r="88" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C88" s="10"/>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="10"/>
+    <row r="89" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C89" s="10"/>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="10"/>
+    <row r="90" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C90" s="10"/>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="10"/>
+    <row r="91" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C91" s="10"/>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="10"/>
+    <row r="92" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C92" s="10"/>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="10"/>
+    <row r="93" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C93" s="10"/>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="10"/>
+    <row r="94" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C94" s="10"/>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="10"/>
+    <row r="95" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C95" s="10"/>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="10"/>
+    <row r="96" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C96" s="10"/>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="10"/>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C97" s="10"/>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="10"/>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C98" s="10"/>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="10"/>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C99" s="10"/>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="10"/>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C100" s="10"/>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="10"/>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C101" s="10"/>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="10"/>
+    <row r="102" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C102" s="10"/>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="10"/>
+    <row r="103" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C103" s="10"/>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="10"/>
+    <row r="104" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C104" s="10"/>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="10"/>
+    <row r="105" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C105" s="10"/>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="10"/>
+    <row r="106" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C106" s="10"/>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="10"/>
+    <row r="107" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C107" s="10"/>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="10"/>
+    <row r="108" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C108" s="10"/>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="10"/>
+    <row r="109" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C109" s="10"/>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="10"/>
+    <row r="110" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C110" s="10"/>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="10"/>
+    <row r="111" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C111" s="10"/>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="10"/>
+    <row r="112" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C112" s="10"/>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="10"/>
+    <row r="113" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C113" s="10"/>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="10"/>
+    <row r="114" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C114" s="10"/>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="10"/>
+    <row r="115" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C115" s="10"/>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="10"/>
+    <row r="116" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C116" s="10"/>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" s="10"/>
+    <row r="117" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C117" s="10"/>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" s="10"/>
+    <row r="118" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C118" s="10"/>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="10"/>
+    <row r="119" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C119" s="10"/>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" s="10"/>
+    <row r="120" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C120" s="10"/>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="10"/>
+    <row r="121" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C121" s="10"/>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="10"/>
+    <row r="122" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C122" s="10"/>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="10"/>
+    <row r="123" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C123" s="10"/>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="10"/>
+    <row r="124" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C124" s="10"/>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="10"/>
+    <row r="125" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C125" s="10"/>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="10"/>
+    <row r="126" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C126" s="10"/>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="10"/>
+    <row r="127" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C127" s="10"/>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" s="10"/>
+    <row r="128" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C128" s="10"/>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" s="10"/>
+    <row r="129" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C129" s="10"/>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" s="10"/>
+    <row r="130" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C130" s="10"/>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="10"/>
+    <row r="131" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C131" s="10"/>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" s="10"/>
+    <row r="132" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C132" s="10"/>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" s="10"/>
+    <row r="133" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C133" s="10"/>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" s="10"/>
+    <row r="134" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C134" s="10"/>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" s="10"/>
+    <row r="135" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C135" s="10"/>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" s="10"/>
+    <row r="136" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C136" s="10"/>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" s="10"/>
+    <row r="137" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C137" s="10"/>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" s="10"/>
+    <row r="138" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C138" s="10"/>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" s="10"/>
+    <row r="139" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C139" s="10"/>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" s="10"/>
+    <row r="140" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C140" s="10"/>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" s="10"/>
+    <row r="141" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C141" s="10"/>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142" s="10"/>
+    <row r="142" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C142" s="10"/>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" s="10"/>
+    <row r="143" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C143" s="10"/>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144" s="10"/>
+    <row r="144" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C144" s="10"/>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A145" s="10"/>
+    <row r="145" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C145" s="10"/>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A146" s="10"/>
+    <row r="146" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C146" s="10"/>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A147" s="10"/>
+    <row r="147" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C147" s="10"/>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" s="10"/>
+    <row r="148" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C148" s="10"/>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149" s="10"/>
+    <row r="149" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C149" s="10"/>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A150" s="10"/>
+    <row r="150" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C150" s="10"/>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A151" s="10"/>
+    <row r="151" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C151" s="10"/>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A152" s="10"/>
+    <row r="152" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C152" s="10"/>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A153" s="10"/>
+    <row r="153" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C153" s="10"/>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A154" s="10"/>
+    <row r="154" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C154" s="10"/>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A155" s="10"/>
+    <row r="155" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C155" s="10"/>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A156" s="10"/>
+    <row r="156" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C156" s="10"/>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A157" s="10"/>
+    <row r="157" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C157" s="10"/>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A158" s="10"/>
+    <row r="158" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C158" s="10"/>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A159" s="10"/>
+    <row r="159" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C159" s="10"/>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A160" s="10"/>
+    <row r="160" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C160" s="10"/>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161" s="10"/>
+    <row r="161" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C161" s="10"/>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162" s="10"/>
+    <row r="162" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C162" s="10"/>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A163" s="10"/>
+    <row r="163" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C163" s="10"/>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A164" s="10"/>
+    <row r="164" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C164" s="10"/>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A165" s="10"/>
+    <row r="165" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C165" s="10"/>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A166" s="10"/>
+    <row r="166" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C166" s="10"/>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A167" s="10"/>
+    <row r="167" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C167" s="10"/>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" s="10"/>
+    <row r="168" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C168" s="10"/>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A169" s="10"/>
+    <row r="169" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C169" s="10"/>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A170" s="10"/>
+    <row r="170" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C170" s="10"/>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A171" s="10"/>
+    <row r="171" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C171" s="10"/>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172" s="10"/>
+    <row r="172" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C172" s="10"/>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A173" s="10"/>
+    <row r="173" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C173" s="10"/>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A174" s="10"/>
+    <row r="174" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C174" s="10"/>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A175" s="10"/>
+    <row r="175" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C175" s="10"/>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A176" s="10"/>
+    <row r="176" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C176" s="10"/>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A177" s="10"/>
+    <row r="177" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C177" s="10"/>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A178" s="10"/>
+    <row r="178" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C178" s="10"/>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A179" s="10"/>
+    <row r="179" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C179" s="10"/>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A180" s="10"/>
+    <row r="180" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C180" s="10"/>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A181" s="10"/>
+    <row r="181" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C181" s="10"/>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A182" s="10"/>
+    <row r="182" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C182" s="10"/>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A183" s="10"/>
+    <row r="183" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C183" s="10"/>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A184" s="10"/>
+    <row r="184" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C184" s="10"/>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A185" s="10"/>
+    <row r="185" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C185" s="10"/>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A186" s="10"/>
+    <row r="186" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C186" s="10"/>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A187" s="10"/>
+    <row r="187" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C187" s="10"/>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A188" s="10"/>
+    <row r="188" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C188" s="10"/>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A189" s="10"/>
+    <row r="189" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C189" s="10"/>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A190" s="10"/>
+    <row r="190" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C190" s="10"/>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A191" s="10"/>
+    <row r="191" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C191" s="10"/>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A192" s="10"/>
+    <row r="192" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C192" s="10"/>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A193" s="10"/>
+    <row r="193" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C193" s="10"/>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A194" s="10"/>
+    <row r="194" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C194" s="10"/>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A195" s="10"/>
+    <row r="195" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C195" s="10"/>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A196" s="10"/>
+    <row r="196" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C196" s="10"/>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A197" s="10"/>
+    <row r="197" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C197" s="10"/>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A198" s="10"/>
+    <row r="198" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C198" s="10"/>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A199" s="10"/>
+    <row r="199" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C199" s="10"/>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A200" s="10"/>
+    <row r="200" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C200" s="10"/>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A201" s="10"/>
+    <row r="201" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C201" s="10"/>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A202" s="10"/>
+    <row r="202" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C202" s="10"/>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A203" s="10"/>
+    <row r="203" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C203" s="10"/>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A204" s="10"/>
+    <row r="204" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C204" s="10"/>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A205" s="10"/>
+    <row r="205" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C205" s="10"/>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A206" s="10"/>
+    <row r="206" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C206" s="10"/>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A207" s="10"/>
+    <row r="207" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C207" s="10"/>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A208" s="10"/>
+    <row r="208" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C208" s="10"/>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A209" s="10"/>
+    <row r="209" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C209" s="10"/>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A210" s="10"/>
+    <row r="210" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C210" s="10"/>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A211" s="10"/>
+    <row r="211" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C211" s="10"/>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A212" s="10"/>
+    <row r="212" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C212" s="10"/>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A213" s="10"/>
+    <row r="213" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C213" s="10"/>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A214" s="10"/>
+    <row r="214" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C214" s="10"/>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A215" s="10"/>
+    <row r="215" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C215" s="10"/>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A216" s="10"/>
+    <row r="216" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C216" s="10"/>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A217" s="10"/>
+    <row r="217" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C217" s="10"/>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A218" s="10"/>
+    <row r="218" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C218" s="10"/>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A219" s="10"/>
+    <row r="219" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C219" s="10"/>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A220" s="10"/>
+    <row r="220" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C220" s="10"/>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A221" s="10"/>
+    <row r="221" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C221" s="10"/>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A222" s="10"/>
+    <row r="222" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C222" s="10"/>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A223" s="10"/>
+    <row r="223" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C223" s="10"/>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A224" s="10"/>
+    <row r="224" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C224" s="10"/>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A225" s="10"/>
+    <row r="225" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C225" s="10"/>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A226" s="10"/>
+    <row r="226" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C226" s="10"/>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A227" s="10"/>
+    <row r="227" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C227" s="10"/>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A228" s="10"/>
+    <row r="228" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C228" s="10"/>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A229" s="10"/>
+    <row r="229" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C229" s="10"/>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A230" s="10"/>
+    <row r="230" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C230" s="10"/>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A231" s="10"/>
+    <row r="231" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C231" s="10"/>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A232" s="10"/>
+    <row r="232" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C232" s="10"/>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A233" s="10"/>
+    <row r="233" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C233" s="10"/>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A234" s="10"/>
+    <row r="234" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C234" s="10"/>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A235" s="10"/>
+    <row r="235" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C235" s="10"/>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A236" s="10"/>
+    <row r="236" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C236" s="10"/>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A237" s="10"/>
+    <row r="237" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C237" s="10"/>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A238" s="10"/>
+    <row r="238" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C238" s="10"/>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A239" s="10"/>
+    <row r="239" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C239" s="10"/>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A240" s="10"/>
+    <row r="240" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C240" s="10"/>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A241" s="10"/>
+    <row r="241" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C241" s="10"/>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A242" s="10"/>
+    <row r="242" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C242" s="10"/>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A243" s="10"/>
+    <row r="243" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C243" s="10"/>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A244" s="10"/>
+    <row r="244" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C244" s="10"/>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A245" s="10"/>
+    <row r="245" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C245" s="10"/>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A246" s="10"/>
+    <row r="246" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C246" s="10"/>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A247" s="10"/>
+    <row r="247" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C247" s="10"/>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A248" s="10"/>
+    <row r="248" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C248" s="10"/>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A249" s="10"/>
+    <row r="249" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C249" s="10"/>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A250" s="10"/>
+    <row r="250" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C250" s="10"/>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A251" s="10"/>
+    <row r="251" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C251" s="10"/>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A252" s="10"/>
+    <row r="252" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C252" s="10"/>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A253" s="10"/>
+    <row r="253" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C253" s="10"/>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A254" s="10"/>
+    <row r="254" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C254" s="10"/>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A255" s="10"/>
+    <row r="255" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C255" s="10"/>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A256" s="10"/>
+    <row r="256" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C256" s="10"/>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A257" s="10"/>
+    <row r="257" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C257" s="10"/>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A258" s="10"/>
+    <row r="258" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C258" s="10"/>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A259" s="10"/>
+    <row r="259" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C259" s="10"/>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A260" s="10"/>
+    <row r="260" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C260" s="10"/>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A261" s="10"/>
+    <row r="261" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C261" s="10"/>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A262" s="10"/>
+    <row r="262" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C262" s="10"/>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A263" s="10"/>
+    <row r="263" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C263" s="10"/>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A264" s="10"/>
+    <row r="264" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C264" s="10"/>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A265" s="10"/>
+    <row r="265" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C265" s="10"/>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A266" s="10"/>
+    <row r="266" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C266" s="10"/>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A267" s="10"/>
+    <row r="267" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C267" s="10"/>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A268" s="10"/>
+    <row r="268" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C268" s="10"/>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A269" s="10"/>
+    <row r="269" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C269" s="10"/>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A270" s="10"/>
+    <row r="270" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C270" s="10"/>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A271" s="10"/>
+    <row r="271" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C271" s="10"/>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A272" s="10"/>
+    <row r="272" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C272" s="10"/>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A273" s="10"/>
+    <row r="273" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C273" s="10"/>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A274" s="10"/>
+    <row r="274" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C274" s="10"/>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A275" s="10"/>
+    <row r="275" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C275" s="10"/>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A276" s="10"/>
+    <row r="276" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C276" s="10"/>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A277" s="10"/>
+    <row r="277" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C277" s="10"/>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A278" s="10"/>
+    <row r="278" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C278" s="10"/>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A279" s="10"/>
+    <row r="279" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C279" s="10"/>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A280" s="10"/>
+    <row r="280" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C280" s="10"/>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A281" s="10"/>
+    <row r="281" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C281" s="10"/>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A282" s="10"/>
+    <row r="282" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C282" s="10"/>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A283" s="10"/>
+    <row r="283" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C283" s="10"/>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A284" s="10"/>
+    <row r="284" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C284" s="10"/>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A285" s="10"/>
+    <row r="285" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C285" s="10"/>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A286" s="10"/>
+    <row r="286" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C286" s="10"/>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A287" s="10"/>
+    <row r="287" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C287" s="10"/>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A288" s="10"/>
+    <row r="288" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C288" s="10"/>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A289" s="10"/>
+    <row r="289" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C289" s="10"/>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A290" s="10"/>
+    <row r="290" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C290" s="10"/>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A291" s="10"/>
+    <row r="291" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C291" s="10"/>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A292" s="10"/>
+    <row r="292" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C292" s="10"/>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A293" s="10"/>
+    <row r="293" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C293" s="10"/>
     </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A294" s="10"/>
+    <row r="294" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C294" s="10"/>
     </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A295" s="10"/>
+    <row r="295" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C295" s="10"/>
     </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A296" s="10"/>
+    <row r="296" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C296" s="10"/>
     </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A297" s="10"/>
+    <row r="297" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C297" s="10"/>
     </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A298" s="10"/>
+    <row r="298" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C298" s="10"/>
     </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A299" s="10"/>
+    <row r="299" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C299" s="10"/>
     </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A300" s="10"/>
+    <row r="300" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C300" s="10"/>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A301" s="10"/>
+    <row r="301" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C301" s="10"/>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A302" s="10"/>
+    <row r="302" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C302" s="10"/>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A303" s="10"/>
+    <row r="303" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C303" s="10"/>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A304" s="10"/>
+    <row r="304" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C304" s="10"/>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A305" s="10"/>
+    <row r="305" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C305" s="10"/>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A306" s="10"/>
+    <row r="306" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C306" s="10"/>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A307" s="10"/>
+    <row r="307" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C307" s="10"/>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A308" s="10"/>
+    <row r="308" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C308" s="10"/>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A309" s="10"/>
+    <row r="309" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C309" s="10"/>
     </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A310" s="10"/>
+    <row r="310" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C310" s="10"/>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A311" s="10"/>
+    <row r="311" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C311" s="10"/>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A312" s="10"/>
+    <row r="312" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C312" s="10"/>
     </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A313" s="10"/>
+    <row r="313" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C313" s="10"/>
     </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A314" s="10"/>
+    <row r="314" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C314" s="10"/>
     </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A315" s="10"/>
+    <row r="315" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C315" s="10"/>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A316" s="10"/>
+    <row r="316" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C316" s="10"/>
     </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A317" s="10"/>
+    <row r="317" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C317" s="10"/>
     </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A318" s="10"/>
+    <row r="318" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C318" s="10"/>
     </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A319" s="10"/>
+    <row r="319" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C319" s="10"/>
     </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A320" s="10"/>
+    <row r="320" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C320" s="10"/>
     </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A321" s="10"/>
+    <row r="321" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C321" s="10"/>
     </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A322" s="10"/>
+    <row r="322" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C322" s="10"/>
     </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A323" s="10"/>
+    <row r="323" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C323" s="10"/>
     </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A324" s="10"/>
+    <row r="324" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C324" s="10"/>
     </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A325" s="10"/>
+    <row r="325" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C325" s="10"/>
     </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A326" s="10"/>
+    <row r="326" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C326" s="10"/>
     </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A327" s="10"/>
+    <row r="327" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C327" s="10"/>
     </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A328" s="10"/>
+    <row r="328" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C328" s="10"/>
     </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A329" s="10"/>
+    <row r="329" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C329" s="10"/>
     </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A330" s="10"/>
+    <row r="330" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C330" s="10"/>
     </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A331" s="10"/>
+    <row r="331" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C331" s="10"/>
     </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A332" s="10"/>
+    <row r="332" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C332" s="10"/>
     </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A333" s="10"/>
+    <row r="333" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C333" s="10"/>
     </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A334" s="10"/>
+    <row r="334" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C334" s="10"/>
     </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A335" s="10"/>
+    <row r="335" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C335" s="10"/>
     </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A336" s="10"/>
+    <row r="336" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C336" s="10"/>
     </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A337" s="10"/>
+    <row r="337" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C337" s="10"/>
     </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A338" s="10"/>
+    <row r="338" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C338" s="10"/>
     </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A339" s="10"/>
+    <row r="339" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C339" s="10"/>
     </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A340" s="10"/>
+    <row r="340" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C340" s="10"/>
     </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A341" s="10"/>
+    <row r="341" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C341" s="10"/>
     </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A342" s="10"/>
+    <row r="342" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C342" s="10"/>
     </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A343" s="10"/>
+    <row r="343" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C343" s="10"/>
     </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A344" s="10"/>
+    <row r="344" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C344" s="10"/>
     </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A345" s="10"/>
+    <row r="345" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C345" s="10"/>
     </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A346" s="10"/>
+    <row r="346" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C346" s="10"/>
     </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A347" s="10"/>
+    <row r="347" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C347" s="10"/>
     </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A348" s="10"/>
+    <row r="348" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C348" s="10"/>
     </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A349" s="10"/>
+    <row r="349" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C349" s="10"/>
     </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A350" s="10"/>
+    <row r="350" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C350" s="10"/>
     </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A351" s="10"/>
+    <row r="351" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C351" s="10"/>
     </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A352" s="10"/>
+    <row r="352" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C352" s="10"/>
     </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A353" s="10"/>
+    <row r="353" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C353" s="10"/>
     </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A354" s="10"/>
+    <row r="354" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C354" s="10"/>
     </row>
-    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A355" s="10"/>
+    <row r="355" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C355" s="10"/>
     </row>
-    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A356" s="10"/>
+    <row r="356" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C356" s="10"/>
     </row>
-    <row r="357" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A357" s="10"/>
+    <row r="357" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C357" s="10"/>
     </row>
-    <row r="358" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A358" s="10"/>
+    <row r="358" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C358" s="10"/>
     </row>
-    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A359" s="10"/>
+    <row r="359" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C359" s="10"/>
     </row>
-    <row r="360" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A360" s="10"/>
+    <row r="360" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C360" s="10"/>
     </row>
-    <row r="361" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A361" s="10"/>
+    <row r="361" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C361" s="10"/>
     </row>
-    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A362" s="10"/>
+    <row r="362" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C362" s="10"/>
     </row>
-    <row r="363" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A363" s="10"/>
+    <row r="363" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C363" s="10"/>
     </row>
-    <row r="364" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A364" s="10"/>
+    <row r="364" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C364" s="10"/>
     </row>
-    <row r="365" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A365" s="10"/>
+    <row r="365" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C365" s="10"/>
     </row>
-    <row r="366" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A366" s="10"/>
+    <row r="366" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C366" s="10"/>
     </row>
-    <row r="367" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A367" s="10"/>
+    <row r="367" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C367" s="10"/>
     </row>
-    <row r="368" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A368" s="10"/>
+    <row r="368" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C368" s="10"/>
     </row>
-    <row r="369" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A369" s="10"/>
+    <row r="369" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C369" s="10"/>
     </row>
-    <row r="370" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A370" s="10"/>
+    <row r="370" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C370" s="10"/>
     </row>
-    <row r="371" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A371" s="10"/>
+    <row r="371" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C371" s="10"/>
     </row>
-    <row r="372" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A372" s="10"/>
+    <row r="372" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C372" s="10"/>
     </row>
-    <row r="373" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A373" s="10"/>
+    <row r="373" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C373" s="10"/>
     </row>
-    <row r="374" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A374" s="10"/>
+    <row r="374" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C374" s="10"/>
     </row>
-    <row r="375" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A375" s="10"/>
+    <row r="375" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C375" s="10"/>
     </row>
-    <row r="376" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A376" s="10"/>
+    <row r="376" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C376" s="10"/>
     </row>
-    <row r="377" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A377" s="10"/>
+    <row r="377" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C377" s="10"/>
     </row>
-    <row r="378" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A378" s="10"/>
+    <row r="378" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C378" s="10"/>
     </row>
-    <row r="379" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A379" s="10"/>
+    <row r="379" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C379" s="10"/>
     </row>
-    <row r="380" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A380" s="10"/>
+    <row r="380" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C380" s="10"/>
     </row>
-    <row r="381" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A381" s="10"/>
+    <row r="381" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C381" s="10"/>
     </row>
-    <row r="382" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A382" s="10"/>
+    <row r="382" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C382" s="10"/>
     </row>
-    <row r="383" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A383" s="10"/>
+    <row r="383" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C383" s="10"/>
     </row>
-    <row r="384" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A384" s="10"/>
+    <row r="384" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C384" s="10"/>
     </row>
-    <row r="385" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A385" s="10"/>
+    <row r="385" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C385" s="10"/>
     </row>
-    <row r="386" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A386" s="10"/>
+    <row r="386" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C386" s="10"/>
     </row>
-    <row r="387" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A387" s="10"/>
+    <row r="387" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C387" s="10"/>
     </row>
-    <row r="388" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A388" s="10"/>
+    <row r="388" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C388" s="10"/>
     </row>
-    <row r="389" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A389" s="10"/>
+    <row r="389" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C389" s="10"/>
     </row>
-    <row r="390" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A390" s="10"/>
+    <row r="390" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C390" s="10"/>
     </row>
-    <row r="391" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A391" s="10"/>
+    <row r="391" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C391" s="10"/>
     </row>
-    <row r="392" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A392" s="10"/>
+    <row r="392" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C392" s="10"/>
     </row>
-    <row r="393" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A393" s="10"/>
+    <row r="393" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C393" s="10"/>
     </row>
-    <row r="394" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A394" s="10"/>
+    <row r="394" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C394" s="10"/>
     </row>
-    <row r="395" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A395" s="10"/>
+    <row r="395" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C395" s="10"/>
     </row>
-    <row r="396" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A396" s="10"/>
+    <row r="396" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C396" s="10"/>
     </row>
-    <row r="397" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A397" s="10"/>
+    <row r="397" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C397" s="10"/>
     </row>
-    <row r="398" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A398" s="10"/>
+    <row r="398" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C398" s="10"/>
     </row>
-    <row r="399" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A399" s="10"/>
+    <row r="399" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C399" s="10"/>
     </row>
-    <row r="400" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A400" s="10"/>
+    <row r="400" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C400" s="10"/>
     </row>
-    <row r="401" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A401" s="10"/>
+    <row r="401" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C401" s="10"/>
     </row>
-    <row r="402" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A402" s="10"/>
+    <row r="402" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C402" s="10"/>
     </row>
-    <row r="403" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A403" s="10"/>
+    <row r="403" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C403" s="10"/>
     </row>
-    <row r="404" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A404" s="10"/>
+    <row r="404" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C404" s="10"/>
     </row>
-    <row r="405" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A405" s="10"/>
+    <row r="405" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C405" s="10"/>
     </row>
-    <row r="406" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A406" s="10"/>
+    <row r="406" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C406" s="10"/>
     </row>
-    <row r="407" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A407" s="10"/>
+    <row r="407" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C407" s="10"/>
     </row>
-    <row r="408" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A408" s="10"/>
+    <row r="408" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C408" s="10"/>
     </row>
-    <row r="409" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A409" s="10"/>
+    <row r="409" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C409" s="10"/>
     </row>
-    <row r="410" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A410" s="10"/>
+    <row r="410" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C410" s="10"/>
     </row>
-    <row r="411" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A411" s="10"/>
+    <row r="411" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C411" s="10"/>
     </row>
-    <row r="412" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A412" s="10"/>
+    <row r="412" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C412" s="10"/>
     </row>
-    <row r="413" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A413" s="10"/>
+    <row r="413" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C413" s="10"/>
     </row>
-    <row r="414" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A414" s="10"/>
+    <row r="414" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C414" s="10"/>
     </row>
-    <row r="415" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A415" s="10"/>
+    <row r="415" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C415" s="10"/>
     </row>
-    <row r="416" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A416" s="10"/>
+    <row r="416" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C416" s="10"/>
     </row>
-    <row r="417" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A417" s="10"/>
+    <row r="417" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C417" s="10"/>
     </row>
-    <row r="418" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A418" s="10"/>
+    <row r="418" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C418" s="10"/>
     </row>
-    <row r="419" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A419" s="10"/>
+    <row r="419" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C419" s="10"/>
     </row>
-    <row r="420" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A420" s="10"/>
+    <row r="420" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C420" s="10"/>
     </row>
-    <row r="421" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A421" s="10"/>
+    <row r="421" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C421" s="10"/>
     </row>
   </sheetData>
@@ -2891,9 +2756,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2911,9 +2776,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>

</xml_diff>